<commit_message>
Adding "Costo tabelle ACI" for template "Modulo A"
</commit_message>
<xml_diff>
--- a/tables/xls/it/61_Mezzi.xlsx
+++ b/tables/xls/it/61_Mezzi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
   <si>
     <t>ORGANIZZAZIONE</t>
   </si>
@@ -39,6 +39,9 @@
     <t>TURNO</t>
   </si>
   <si>
+    <t>COSTO TABELLE ACI</t>
+  </si>
+  <si>
     <t>KM INIZIO MISSIONE</t>
   </si>
   <si>
@@ -81,154 +84,160 @@
     <t>Nome (abbrev.)</t>
   </si>
   <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Elenco di valori (separati da virgola)</t>
+  </si>
+  <si>
+    <t>Dim. massima</t>
+  </si>
+  <si>
+    <t>Obbligatorio</t>
+  </si>
+  <si>
+    <t>Valore predefinito</t>
+  </si>
+  <si>
+    <t>Sola lettura</t>
+  </si>
+  <si>
+    <t>Visibile</t>
+  </si>
+  <si>
+    <t>Forza</t>
+  </si>
+  <si>
+    <t>Valore unico</t>
+  </si>
+  <si>
+    <t>Opzioni campo</t>
+  </si>
+  <si>
+    <t>Scheda dati per suggerimento</t>
+  </si>
+  <si>
+    <t>Campo suggerimento</t>
+  </si>
+  <si>
+    <t>Testo aiuto</t>
+  </si>
+  <si>
+    <t>Configurazione Scheda Dati</t>
+  </si>
+  <si>
+    <t>Nome Scheda Dati</t>
+  </si>
+  <si>
+    <t>Descrizione Scheda Dati</t>
+  </si>
+  <si>
+    <t>Ordina scheda per</t>
+  </si>
+  <si>
+    <t>Direzione ordinamento</t>
+  </si>
+  <si>
+    <t>Consenti modifiche</t>
+  </si>
+  <si>
+    <t>Consenti inserimenti</t>
+  </si>
+  <si>
+    <t>Consenti cancellazioni</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Testo</t>
+  </si>
+  <si>
+    <t>Sì</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>MEZZI ATTESI</t>
+  </si>
+  <si>
+    <t>autofocus</t>
+  </si>
+  <si>
+    <t>Testo - Elenco di valori</t>
+  </si>
+  <si>
+    <t>n.d.,NO,SI</t>
+  </si>
+  <si>
+    <t>n.d.,No,Aperto,Chiuso</t>
+  </si>
+  <si>
+    <t>Numero Intero</t>
+  </si>
+  <si>
+    <t>ultimo valore</t>
+  </si>
+  <si>
+    <t>COSTO ACI</t>
+  </si>
+  <si>
+    <t>Numero Decimale</t>
+  </si>
+  <si>
     <t>DATA/ORA REG.</t>
   </si>
   <si>
+    <t>Data e ora</t>
+  </si>
+  <si>
+    <t>adesso</t>
+  </si>
+  <si>
     <t>DATA/ORA USCITA</t>
   </si>
   <si>
+    <t>IN ATTESA DI SERVIZIO</t>
+  </si>
+  <si>
+    <t>Numero Intero progressivo</t>
+  </si>
+  <si>
     <t>DATA INIZIO ATTEST.</t>
   </si>
   <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>oggi</t>
+  </si>
+  <si>
     <t>DATA FINE ATTEST.</t>
   </si>
   <si>
     <t>COD. ORGANIZZAZIONE</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Testo</t>
-  </si>
-  <si>
-    <t>Testo - Elenco di valori</t>
-  </si>
-  <si>
-    <t>Numero Intero</t>
-  </si>
-  <si>
-    <t>Data e ora</t>
-  </si>
-  <si>
-    <t>Numero Intero progressivo</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Elenco di valori (separati da virgola)</t>
-  </si>
-  <si>
-    <t>n.d.,NO,SI</t>
-  </si>
-  <si>
-    <t>n.d.,No,Aperto,Chiuso</t>
-  </si>
-  <si>
-    <t>Dim. massima</t>
-  </si>
-  <si>
-    <t>Obbligatorio</t>
-  </si>
-  <si>
-    <t>Sì</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Valore predefinito</t>
-  </si>
-  <si>
-    <t>ultimo valore</t>
-  </si>
-  <si>
-    <t>adesso</t>
-  </si>
-  <si>
-    <t>IN ATTESA DI SERVIZIO</t>
-  </si>
-  <si>
-    <t>oggi</t>
-  </si>
-  <si>
-    <t>Sola lettura</t>
-  </si>
-  <si>
-    <t>Visibile</t>
-  </si>
-  <si>
-    <t>Forza</t>
-  </si>
-  <si>
-    <t>Valore unico</t>
-  </si>
-  <si>
-    <t>Opzioni campo</t>
-  </si>
-  <si>
-    <t>autofocus</t>
-  </si>
-  <si>
-    <t>Scheda dati per suggerimento</t>
-  </si>
-  <si>
-    <t>MEZZI ATTESI</t>
-  </si>
-  <si>
-    <t>Campo suggerimento</t>
-  </si>
-  <si>
-    <t>Testo aiuto</t>
-  </si>
-  <si>
-    <t>Configurazione Scheda Dati</t>
+    <t>MEZZI</t>
+  </si>
+  <si>
+    <t>Mezzi</t>
+  </si>
+  <si>
+    <t>Crescente</t>
+  </si>
+  <si>
+    <t>RISORSE</t>
   </si>
   <si>
     <t>Elenco segnalibri</t>
   </si>
   <si>
-    <t>Nome Scheda Dati</t>
-  </si>
-  <si>
-    <t>MEZZI</t>
-  </si>
-  <si>
     <t>Mezzi in servizio</t>
   </si>
   <si>
     <t>"DATA/ORA USCITA" vuoto</t>
-  </si>
-  <si>
-    <t>Descrizione Scheda Dati</t>
-  </si>
-  <si>
-    <t>Mezzi</t>
-  </si>
-  <si>
-    <t>Ordina scheda per</t>
-  </si>
-  <si>
-    <t>Direzione ordinamento</t>
-  </si>
-  <si>
-    <t>Crescente</t>
-  </si>
-  <si>
-    <t>Consenti modifiche</t>
-  </si>
-  <si>
-    <t>Consenti inserimenti</t>
-  </si>
-  <si>
-    <t>Consenti cancellazioni</t>
-  </si>
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>RISORSE</t>
   </si>
 </sst>
 </file>
@@ -252,10 +261,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -266,7 +272,7 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,11 +569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,7 +581,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,13 +638,16 @@
       </c>
       <c r="S1" t="s">
         <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -647,15 +656,16 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,7 +673,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -721,10 +731,13 @@
       <c r="T1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -748,45 +761,48 @@
         <v>8</v>
       </c>
       <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
         <v>11</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>12</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>13</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>14</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>15</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>16</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>19</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>20</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>21</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>29</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>30</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -810,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="J3" t="s">
         <v>8</v>
@@ -819,107 +835,113 @@
         <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="N3" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="O3" t="s">
         <v>13</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="Q3" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="S3" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="T3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="N4" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="O4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="Q4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="R4" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="S4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="T4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>44</v>
+      </c>
+      <c r="U4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -935,10 +957,11 @@
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>255</v>
@@ -997,72 +1020,78 @@
       <c r="T6">
         <v>255</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="N7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="O7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="P7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="Q7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="S7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="T7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+        <v>45</v>
+      </c>
+      <c r="U7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -1071,168 +1100,175 @@
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
-      <c r="L8" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8"/>
-      <c r="N8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8"/>
-      <c r="P8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8"/>
+      <c r="L8"/>
+      <c r="M8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8"/>
+      <c r="O8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P8"/>
+      <c r="Q8" t="s">
+        <v>64</v>
+      </c>
       <c r="R8"/>
       <c r="S8"/>
       <c r="T8"/>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="M9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="O9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="P9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="Q9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="R9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="S9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="T9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>46</v>
+      </c>
+      <c r="U9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="M10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="N10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="O10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="P10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="Q10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="R10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="S10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="T10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>45</v>
+      </c>
+      <c r="U10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -1246,80 +1282,84 @@
       <c r="Q11"/>
       <c r="R11"/>
       <c r="S11"/>
-      <c r="T11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="T11"/>
+      <c r="U11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="M12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="N12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="O12" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="P12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="Q12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="R12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="S12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="T12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>46</v>
+      </c>
+      <c r="U12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -1337,31 +1377,32 @@
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13"/>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1369,24 +1410,25 @@
       <c r="L14"/>
       <c r="M14"/>
       <c r="N14"/>
-      <c r="O14" t="s">
-        <v>52</v>
-      </c>
-      <c r="P14"/>
+      <c r="O14"/>
+      <c r="P14" t="s">
+        <v>47</v>
+      </c>
       <c r="Q14"/>
-      <c r="R14" t="s">
-        <v>52</v>
-      </c>
+      <c r="R14"/>
       <c r="S14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="T14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+        <v>47</v>
+      </c>
+      <c r="U14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1415,24 +1457,25 @@
       <c r="L15"/>
       <c r="M15"/>
       <c r="N15"/>
-      <c r="O15" t="s">
-        <v>13</v>
-      </c>
-      <c r="P15"/>
+      <c r="O15"/>
+      <c r="P15" t="s">
+        <v>14</v>
+      </c>
       <c r="Q15"/>
-      <c r="R15" t="s">
-        <v>16</v>
-      </c>
+      <c r="R15"/>
       <c r="S15" t="s">
         <v>17</v>
       </c>
       <c r="T15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -1453,80 +1496,81 @@
       <c r="R16"/>
       <c r="S16"/>
       <c r="T16"/>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16"/>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
         <v>70</v>
@@ -1536,7 +1580,7 @@
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -1545,5 +1589,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>